<commit_message>
Changes testing data and changed test case file name
</commit_message>
<xml_diff>
--- a/Loan Eligibility Data.xlsx
+++ b/Loan Eligibility Data.xlsx
@@ -470,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,26 +559,6 @@
       </c>
       <c r="F4" s="3">
         <v>66251</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>80000</v>
-      </c>
-      <c r="B5">
-        <v>20</v>
-      </c>
-      <c r="C5">
-        <v>6.5</v>
-      </c>
-      <c r="D5">
-        <v>10000</v>
-      </c>
-      <c r="E5">
-        <v>4023750</v>
-      </c>
-      <c r="F5" s="3">
-        <v>30000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>